<commit_message>
添加 dotnet  watch  run  和 扩展sql，添加到  xml中
</commit_message>
<xml_diff>
--- a/Document/数据库设计.xlsx
+++ b/Document/数据库设计.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="125">
   <si>
     <t>列名</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t>varchar(50)</t>
+  </si>
+  <si>
+    <t>测试表(t_demo)</t>
   </si>
 </sst>
 </file>
@@ -919,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F140"/>
+  <dimension ref="A1:F165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="F162" sqref="F162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2936,26 +2939,358 @@
         <v>31</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
-      <c r="B140" s="5" t="s">
+    <row r="139" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="140" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A140" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B140" s="7"/>
+      <c r="C140" s="7"/>
+      <c r="D140" s="7"/>
+      <c r="E140" s="7"/>
+      <c r="F140" s="8"/>
+    </row>
+    <row r="141" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A141" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A142" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D142" s="4"/>
+      <c r="E142" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F142" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A143" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D143" s="4"/>
+      <c r="E143" s="4"/>
+      <c r="F143" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A144" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C144" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D144" s="4"/>
+      <c r="E144" s="4"/>
+      <c r="F144" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A145" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D145" s="4"/>
+      <c r="E145" s="4"/>
+      <c r="F145" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A146" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D146" s="4"/>
+      <c r="E146" s="4"/>
+      <c r="F146" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A147" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C147" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D147" s="4"/>
+      <c r="E147" s="4"/>
+      <c r="F147" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A148" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B148" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D148" s="4">
+        <v>0</v>
+      </c>
+      <c r="E148" s="4"/>
+      <c r="F148" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A149" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D149" s="4"/>
+      <c r="E149" s="4"/>
+      <c r="F149" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A150" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B150" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D150" s="4">
+        <v>0</v>
+      </c>
+      <c r="E150" s="4"/>
+      <c r="F150" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A151" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C151" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D151" s="4">
+        <v>0</v>
+      </c>
+      <c r="E151" s="4"/>
+      <c r="F151" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A152" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B152" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C152" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D152" s="4">
+        <v>0</v>
+      </c>
+      <c r="E152" s="4"/>
+      <c r="F152" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A153" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B153" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C153" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D153" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E153" s="4"/>
+      <c r="F153" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A154" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C154" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D154" s="4"/>
+      <c r="E154" s="4"/>
+      <c r="F154" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A155" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C155" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D155" s="4"/>
+      <c r="E155" s="4"/>
+      <c r="F155" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A156" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C156" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D156" s="4"/>
+      <c r="E156" s="4"/>
+      <c r="F156" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A157" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B157" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C157" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D157" s="4"/>
+      <c r="E157" s="4"/>
+      <c r="F157" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A158" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C158" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D158" s="4"/>
+      <c r="E158" s="4"/>
+      <c r="F158" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A159" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C159" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D159" s="4"/>
+      <c r="E159" s="4"/>
+      <c r="F159" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="165" spans="2:3">
+      <c r="B165" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C140" s="5" t="s">
+      <c r="C165" s="5" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A140:F140"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A70:F70"/>
     <mergeCell ref="A89:F89"/>
     <mergeCell ref="A99:F99"/>
     <mergeCell ref="A110:F110"/>
     <mergeCell ref="A120:F120"/>
     <mergeCell ref="A130:F130"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A70:F70"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>